<commit_message>
Finally fixed right moments of inertia
</commit_message>
<xml_diff>
--- a/measured_params.xlsx
+++ b/measured_params.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rogiers\Documents\GitHub\8barlinkage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kuleuven-my.sharepoint.com/personal/martijn_spaepen_student_kuleuven_be/Documents/KU Leuven/3/Semester 2/Beweging/8barlinkage/8barlinkage/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_0C602F1C0E6E7BE4F8FECC4310974DDE816AF09E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2760" yWindow="1335" windowWidth="17280" windowHeight="8970"/>
+    <workbookView minimized="1" xWindow="2760" yWindow="1332" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -160,11 +161,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
@@ -313,11 +314,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,10 +330,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,19 +648,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="8.875" style="10"/>
+    <col min="3" max="3" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
+    <row r="1" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -675,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1">
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -692,7 +688,7 @@
         <v>0.14166000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -709,7 +705,7 @@
         <v>0.70548</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -722,11 +718,11 @@
       <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="6">
         <v>1.3367</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -743,7 +739,7 @@
         <v>0.20319999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -760,7 +756,7 @@
         <v>0.43130000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -771,7 +767,7 @@
         <v>6.2862</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -782,7 +778,7 @@
         <v>2.5442</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -793,7 +789,7 @@
         <v>4.3380000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -804,7 +800,7 @@
         <v>5.7115999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -815,7 +811,7 @@
         <v>8.3091000000000008</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -826,7 +822,7 @@
         <v>2.9988000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -837,7 +833,7 @@
         <v>7.3620000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -848,7 +844,7 @@
         <v>9.1835000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -859,7 +855,7 @@
         <v>3.6602999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -870,7 +866,7 @@
         <v>1.3446</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>38</v>
       </c>

</xml_diff>